<commit_message>
adjust bible verse pause
</commit_message>
<xml_diff>
--- a/src/main/resources/2-year-reading-plan.xlsx
+++ b/src/main/resources/2-year-reading-plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuchaochih/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuchaochih/Documents/GitHub/churchrpg/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA13FB8-4082-2E45-B2DC-8CC6CF697DBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79AB7E4-D70E-6D4F-80F6-DBB63B19BFB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{AD0F1010-94C3-CC46-ACCF-B31ED1A61D11}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD0F1010-94C3-CC46-ACCF-B31ED1A61D11}"/>
   </bookViews>
   <sheets>
     <sheet name="1st year" sheetId="1" r:id="rId1"/>
@@ -4938,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674051FE-8747-BD41-AC70-AF4A4AAD628B}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView zoomScale="276" zoomScaleNormal="276" workbookViewId="0">
-      <selection activeCell="D60" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="276" zoomScaleNormal="276" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10695,8 +10695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376C2656-7156-4B44-9B38-3D634EAD4E7F}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13548,11 +13548,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="M36:N36"/>
     <mergeCell ref="P36:Q36"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:B2"/>
@@ -13561,6 +13556,11 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="M36:N36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13570,7 +13570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76A2F42-F63A-B945-8DEB-968CC22EC9FC}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -16430,11 +16430,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="M36:N36"/>
     <mergeCell ref="P36:Q36"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="A2:B2"/>
@@ -16443,6 +16438,11 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="M36:N36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
if title contain html tag, parsing entire rpg article fails
</commit_message>
<xml_diff>
--- a/src/main/resources/2-year-reading-plan.xlsx
+++ b/src/main/resources/2-year-reading-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuchaochih/Documents/GitHub/churchrpg/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79AB7E4-D70E-6D4F-80F6-DBB63B19BFB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6BF92C-6D89-0748-AE01-382AA0E5B049}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{AD0F1010-94C3-CC46-ACCF-B31ED1A61D11}"/>
+    <workbookView xWindow="1020" yWindow="18000" windowWidth="28800" windowHeight="18000" xr2:uid="{AD0F1010-94C3-CC46-ACCF-B31ED1A61D11}"/>
   </bookViews>
   <sheets>
     <sheet name="1st year" sheetId="1" r:id="rId1"/>
@@ -4938,7 +4938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674051FE-8747-BD41-AC70-AF4A4AAD628B}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="276" zoomScaleNormal="276" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="276" zoomScaleNormal="276" workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>

</xml_diff>